<commit_message>
added SpokenLanguageExpression and Swallowing observation
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-splasch-SpokenLanguageComprehension.xlsx
+++ b/output/StructureDefinition-splasch-SpokenLanguageComprehension.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2021-11-24T17:18:22-05:00</t>
+    <t>2021-11-30T03:26:11-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -84,7 +84,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>An exchange of cognitive status data for a patient.</t>
+    <t>An exchange of spoken language comprehension data for a patient.</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>

<commit_message>
combined code systems and value sets into a single file based on Cognitive Status IG example. This may change, but I'm comitting here to avoid losing progress.
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-splasch-SpokenLanguageComprehension.xlsx
+++ b/output/StructureDefinition-splasch-SpokenLanguageComprehension.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2021-11-30T03:26:11-05:00</t>
+    <t>2021-12-06T15:18:55-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -651,7 +651,7 @@
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
   &lt;coding&gt;
-    &lt;system value="http://hl7.org/fhir/us/pacio-splasch/CodeSystem/SPLASCHObservationCategory"/&gt;
+    &lt;system value="http://hl7.org/fhir/us/pacio-splasch/CodeSystem/pacio-splasch-cs"/&gt;
     &lt;code value="spoken-language-comprehension"/&gt;
   &lt;/coding&gt;
 &lt;/valueCodeableConcept&gt;</t>

</xml_diff>